<commit_message>
Creates pyproject task to run fake_data. Update fake_data script to add fake incorrect and correct data load
</commit_message>
<xml_diff>
--- a/data/sales_data.xlsx
+++ b/data/sales_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,100 +472,100 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>pjackson@example.com</t>
+          <t>sbullock@example.org</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45668</v>
+        <v>45528</v>
       </c>
       <c r="C2" t="n">
-        <v>819.8</v>
+        <v>236.5</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>b2b</t>
+          <t>retail</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>zbell@example.org</t>
+          <t>danaacevedo@example.org</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45609</v>
+        <v>45687</v>
       </c>
       <c r="C3" t="n">
-        <v>197.36</v>
+        <v>209.68</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Themselves</t>
+          <t>When</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>b2b</t>
+          <t>online</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>harrisbrian@example.com</t>
+          <t>robertskelly@example.net</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45407</v>
+        <v>45638</v>
       </c>
       <c r="C4" t="n">
-        <v>198.58</v>
+        <v>68.23</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Property</t>
+          <t>Why</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>retail</t>
+          <t>b2b</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>joannabell@example.org</t>
+          <t>devin10@example.net</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45417</v>
+        <v>45441</v>
       </c>
       <c r="C5" t="n">
-        <v>921.74</v>
+        <v>915.1900000000001</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>Tough</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -576,74 +576,74 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>alexmartinez@example.net</t>
+          <t>tinataylor@example.com</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45493</v>
+        <v>45373</v>
       </c>
       <c r="C6" t="n">
-        <v>803.16</v>
+        <v>335.82</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Staff</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>b2b</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>austingordon@example.net</t>
+          <t>boneal@example.org</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45667</v>
+        <v>45643</v>
       </c>
       <c r="C7" t="n">
-        <v>214.12</v>
+        <v>787.5</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Memory</t>
+          <t>Money</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>b2b</t>
+          <t>online</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>dennishayes@example.com</t>
+          <t>xsmith@example.org</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45519</v>
+        <v>45421</v>
       </c>
       <c r="C8" t="n">
-        <v>854.87</v>
+        <v>132.95</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Since</t>
+          <t>Pressure</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -654,22 +654,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>cunderwood@example.net</t>
+          <t>davidharding@example.com</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45620</v>
+        <v>45509</v>
       </c>
       <c r="C9" t="n">
-        <v>829.37</v>
+        <v>326.88</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Activity</t>
+          <t>News</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -680,50 +680,310 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>wendy15@example.net</t>
+          <t>cjohnson@example.net</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45514</v>
+        <v>45584</v>
       </c>
       <c r="C10" t="n">
-        <v>883.11</v>
+        <v>156.27</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Say</t>
+          <t>Daughter</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>retail</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>calebrobbins@example.org</t>
+          <t>tlove@example.com</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45459</v>
+        <v>45590</v>
       </c>
       <c r="C11" t="n">
-        <v>679.0599999999999</v>
+        <v>181.99</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>News</t>
+          <t>Fact</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="F11" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>williamsmichelle@example.net</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>45379</v>
+      </c>
+      <c r="C12" t="n">
+        <v>176.09</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Before</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>rthomas@example.net</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>45651</v>
+      </c>
+      <c r="C13" t="n">
+        <v>488.08</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>14</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>b2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>hawkinsjohnny@example.net</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>45695</v>
+      </c>
+      <c r="C14" t="n">
+        <v>922.24</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Add</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>93</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>b2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>john98@example.net</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>45616</v>
+      </c>
+      <c r="C15" t="n">
+        <v>975.3099999999999</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Often</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>94</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>retail</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>mayerdiana@example.org</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>45575</v>
+      </c>
+      <c r="C16" t="n">
+        <v>310.58</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Interesting</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>15</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>julie52@example.org</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>45558</v>
+      </c>
+      <c r="C17" t="n">
+        <v>219.21</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>35</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>retail</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>davidwalker@example.com</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="C18" t="n">
+        <v>404.18</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Partner</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>29</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>tdiaz@example.org</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>45570</v>
+      </c>
+      <c r="C19" t="n">
+        <v>452.66</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>100</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>b2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>alyssa08@example.org</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>45501</v>
+      </c>
+      <c r="C20" t="n">
+        <v>411.06</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Early</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>66</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>retail</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>fishersamuel@example.org</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>45480</v>
+      </c>
+      <c r="C21" t="n">
+        <v>263.35</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Responsibility</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>31</v>
+      </c>
+      <c r="F21" t="inlineStr">
         <is>
           <t>b2b</t>
         </is>

</xml_diff>